<commit_message>
Atualização automática de SAO_MARCOS.xlsx
</commit_message>
<xml_diff>
--- a/SAO_MARCOS.xlsx
+++ b/SAO_MARCOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82F4E9D7-B0E2-4AC9-BA83-836CBE6B9577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0842FA7F-2CC6-4863-9315-17FD7F0DC5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1197,7 +1197,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{EDFDEF3A-F35F-40AE-999B-469971C6C969}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{EFEAC569-9E72-4ACA-899F-AE9240D285F3}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1227,10 +1227,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13A46323-01E7-4896-B382-657AA394698B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9403748-3679-444A-A293-62F985A660D7}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1268,7 +1268,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75925767-6C67-4803-9463-C64A9A761D39}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{529F1006-E2E8-424C-A08C-9C755BB08BB1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1331,7 +1331,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77A807C8-CC19-4509-9260-A0EC3A511ED6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1890587A-48FC-4C81-A3A9-DBC1273492C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1350,7 +1350,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6353AC17-1ABB-B193-D4C0-5AC038CA3A9C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBB0905D-2434-7B7A-B9D2-6272AE309357}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1399,7 +1399,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36469E0B-FFF9-DE25-225B-DF2CFC2C7925}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D84F0A02-1C7D-1645-44C5-213473CECCC2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1418,7 +1418,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FBAABC5-4EAF-5932-17CF-F9E241F9F976}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A785B58F-6A95-8C70-01C3-FA1CBA975957}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1449,7 +1449,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAB5C5D6-B612-9B0B-3C2C-82DB5CD03869}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC64D7DB-79A1-A85B-1FBC-B954B2E10BFA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1480,7 +1480,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4667101C-E2FF-D06A-57F4-756E2EE38CD9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A0AE74A-BF1F-A55F-7F62-238F8E347399}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1523,7 +1523,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E8E171D-47C9-4F05-B698-4FA6CDEFDBA0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6F8F8BF-E90B-4033-9E79-F212DDE5413D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1561,7 +1561,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03912699-3348-4F33-940F-4B0675319272}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6092418-F733-454C-A503-9737933AC6A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1604,7 +1604,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F92CA0CA-5E44-41DD-A7F6-391E2B8F2733}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC5B266D-FFE4-408C-9AE1-CEFECAC2F08E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1917,7 +1917,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC88EE2-434E-476B-82C2-E33B098621DC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D7E44E1-4130-40BB-8B3E-CADCDBC2D083}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>